<commit_message>
added the runtime distribution
</commit_message>
<xml_diff>
--- a/metrics/results.xlsx
+++ b/metrics/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pujas\Courses\Program_Analysis\ProgramAnalysisProject\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B05A759-15B7-4F96-878A-1E2F6DD1054B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC37680-60D8-40F3-B8E1-E6A64E60F2A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A0767390-89B2-45B0-90FC-3CDDCB71A2F6}"/>
   </bookViews>
@@ -163,6 +163,1702 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Runtime Distribution</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Intervals</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$B$64</c:f>
+              <c:strCache>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>alwaysThrows1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>alwaysThrows1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>always Throws1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>alwaysThrows1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>alwaysThrows1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>alwaysThrows2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>alwaysThrows2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>alwaysThrows2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>alwaysThrows2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>alwaysThrows2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>alwaysThrows3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>alwaysThrows3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>alwaysThrows3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>alwaysThrows3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>alwaysThrows3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>alwaysThrows4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>alwaysThrows4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>alwaysThrows4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>alwaysThrows4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>alwaysThrows4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>alwaysThrows5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>alwaysThrows5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>alwaysThrows5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>alwaysThrows5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>alwaysThrows5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>dependsOnLattice1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>dependsOnLattice1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>dependsOnLattice1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>dependsOnLattice1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>dependsOnLattice1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>dependsOnLattice2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>dependsOnLattice2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>dependsOnLattice2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>dependsOnLattice2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>dependsOnLattice2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>dependsOnLattice3</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>dependsOnLattice3</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>dependsOnLattice3</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>dependsOnLattice3</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>dependsOnLattice3</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>bubbleSort</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>bubbleSort</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>bubbleSort</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>bubbleSort</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>bubbleSort</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>insertionSort</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>insertionSort</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>insertionSort</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>insertionSort</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>insertionSort</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>selectionSort</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>selectionSort</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>selectionSort</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>selectionSort</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>selectionSort</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>binarySearch</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>binarySearch</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>binarySearch</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>binarySearch</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>binarySearch</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$64</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="63"/>
+                <c:pt idx="0">
+                  <c:v>6.6360800061374903E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.4930099993944099E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.0593000389635494E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.2274200152605703E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.8754999898373997E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.3867299780249498E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.1401899866759701E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.0469600334763499E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.9824900198727801E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.52902998961508E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.15491389995440799</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.13842049986124</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.158864200115203</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.165001400280743</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.135727200191468</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.8096099868416703E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.3219699990004301E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.7304300125688301E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.1478400360792799E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.2127600181847797E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.14845120022073299</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.117030899971723</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.14595669973641601</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.14810580015182401</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.151557999663054</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.4219000078737694E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9.4578800257295301E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8.86567998677492E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8.8165000081062303E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>9.0519200079143006E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.7068999614566502E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.6638399828225298E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6.2147600110620198E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>9.3210299964994095E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8.9429300278425203E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>6.8886300083249793E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>7.4653400108218096E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>6.2306399922817897E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>6.1169200111180502E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>7.0768000092357397E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.19095239974558301</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.18886539991945001</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.21165519999340099</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.179210200440138</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.179868099745363</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.29493749979883399</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.32261289982125102</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.28112389985471897</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.30278299981728102</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.25625029997900101</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.36150539992377101</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.38655569963157099</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.40245759999379499</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.38906510034575997</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.37000430002808499</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.16721219988539801</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.190172700211405</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.16825329978018999</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.184962300118058</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.16022149985656101</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.14118514501024007</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-504E-403D-906C-97C53E3A648E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pentagon</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$B$64</c:f>
+              <c:strCache>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>alwaysThrows1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>alwaysThrows1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>always Throws1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>alwaysThrows1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>alwaysThrows1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>alwaysThrows2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>alwaysThrows2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>alwaysThrows2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>alwaysThrows2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>alwaysThrows2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>alwaysThrows3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>alwaysThrows3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>alwaysThrows3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>alwaysThrows3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>alwaysThrows3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>alwaysThrows4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>alwaysThrows4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>alwaysThrows4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>alwaysThrows4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>alwaysThrows4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>alwaysThrows5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>alwaysThrows5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>alwaysThrows5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>alwaysThrows5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>alwaysThrows5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>dependsOnLattice1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>dependsOnLattice1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>dependsOnLattice1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>dependsOnLattice1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>dependsOnLattice1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>dependsOnLattice2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>dependsOnLattice2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>dependsOnLattice2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>dependsOnLattice2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>dependsOnLattice2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>dependsOnLattice3</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>dependsOnLattice3</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>dependsOnLattice3</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>dependsOnLattice3</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>dependsOnLattice3</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>bubbleSort</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>bubbleSort</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>bubbleSort</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>bubbleSort</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>bubbleSort</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>insertionSort</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>insertionSort</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>insertionSort</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>insertionSort</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>insertionSort</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>selectionSort</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>selectionSort</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>selectionSort</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>selectionSort</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>selectionSort</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>binarySearch</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>binarySearch</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>binarySearch</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>binarySearch</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>binarySearch</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$64</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="63"/>
+                <c:pt idx="0">
+                  <c:v>9.8151399753987706E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.102119099814444</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.110233900137245</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.6117499750107499E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.9195699673145996E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1721799857914399E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.8202400077134301E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.7534099761396601E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.1704800203442497E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.69785998389124E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.242161899805068</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.222419300116598</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.22239070013165399</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.21706089982762899</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.22809049999341299</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.8950999993830905E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.1246199999004602E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.4357199929654598E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.2333500236272798E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.0439500026404802E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.24094509985297899</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.249408800154924</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.23966260021552399</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.23950259992852799</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.25614660000428502</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.180711699649691</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.188400299753993</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.18374580005183799</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.19210830004885701</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.17673420021310399</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.11731779994443001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.102583699859678</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.118315000087022</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.103535200003534</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.118187200278043</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.12107429979369</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.12099450035020699</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.11669320007786101</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.12501579988747799</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.11779629997909</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.40232980018481601</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.40950899990275502</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.42895799968391601</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.45072060031816302</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.37518400000408197</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.94418620038777501</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.89997030002996303</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.0174695001915</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.94899489963427097</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.955998999997973</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2.39971900032833</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2.3562293001450598</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2.3764769998378998</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2.4358846000395702</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2.4069798998534599</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.25120760034769701</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.30973049998283297</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.327129299752414</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.31871390016749501</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.29700289992615497</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.4282114049963025</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-504E-403D-906C-97C53E3A648E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1310614160"/>
+        <c:axId val="1410136336"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1310614160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1410136336"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1410136336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1310614160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90633BD1-1CBD-52F9-8FC5-C7E88B989589}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -464,8 +2160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5300386F-2806-4E3C-BA1E-98E00AE12611}">
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1421,5 +3117,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>